<commit_message>
Fewshot and Methods experiments fully completed
</commit_message>
<xml_diff>
--- a/experiments/results/fewshot_eval.xlsx
+++ b/experiments/results/fewshot_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F87E73-7D7D-4104-AE7A-BF6BD944663A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754F42F8-213D-4439-A98B-E95DA3A0C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>query_id</t>
   </si>
@@ -402,6 +402,1508 @@
   </si>
   <si>
     <t>only_schema</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?disease
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor .
+    ?descriptor cmeo:has_value ?disease .
+    FILTER(CONTAINS(LCASE(?disease), "diabetes"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?disease_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor .
+    ?descriptor cmeo:has_value ?disease_label .
+    FILTER(CONTAINS(LCASE(?disease_label), "coronary heart disease"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?variable_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:study_design_variable_specification ;
+           dc:identifier ?id ;
+           ro:has_part ?variable .
+    FILTER(CONTAINS(LCASE(STR(?id)), "time-chf"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?drugVariableCount)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:study_design_variable_specification ;
+           dc:identifier "time-chf"^^xsd:string ;
+           ro:has_part ?variable .
+    ?variable cmeo:has_value ?value .
+    FILTER(CONTAINS(LCASE(STR(?value)), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?trial ?protocol
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?trial a cmeo:randomized_controlled_trial ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor ;
+           rdfs:label ?study_label .
+    ?descriptor cmeo:has_value ?condition_value .
+    FILTER(CONTAINS(LCASE(STR(?condition_value)), "heart failure"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT ?study ?populationCharacteristic ?value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           ro:has_part ?eligibilityCriterion .
+    ?eligibilityCriterion a obi:eligibility_criterion ;
+           ro:has_part ?inclusionCriterion .
+    ?inclusionCriterion a obi:inclusion_criterion ;
+           ro:has_part ?populationCharacteristic .
+    ?populationCharacteristic cmeo:has_value ?value .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study ?study_label
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           rdfs:label ?study_label ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility_criterion, ?intervention, ?comparator, ?outcome .
+    ?eligibility_criterion a obi:eligibility_criterion .
+    ?intervention a cmeo:intervention_specification .
+    ?comparator a cmeo:comparator_specification .
+    ?outcome a cmeo:outcome_specification .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           iao:is_about ?descriptor ;
+           ro:has_part ?data_policy , ?data_modifier .
+    ?data_policy a duo:data_use_permission ;
+                 rdfs:label "disease specific research"^^xsd:string .
+    ?data_modifier a duo:data_use_modifier ;
+                   rdfs:label "ethics approval required"^^xsd:string .
+    ?descriptor cmeo:has_value ?disease .
+    FILTER(CONTAINS(LCASE(?disease), "congestive heart failure"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name;
+                ro:concretizes ?study_design.
+          ?study_design  ro:has_part ?protocol .
+         # Primary purpose specification
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         # Inclusion criteria pattern (optional)
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         # Filter: Only include studies where the primary purpose or inclusion criteria contain "diabetes"
+         FILTER( regex(lcase(str(?purpose)), 'diabetes') ||
+           (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'diabetes'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name;
+                ro:concretizes ?study_design.
+          ?study_design  ro:has_part ?protocol .
+         # Primary purpose specification
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         # Inclusion criteria pattern (optional)
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         # Filter for diabetes disease
+         FILTER( regex(lcase(str(?purpose)), 'diabetes') ||
+           (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'diabetes'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study a obi:study_design_execution ;
+               dc:identifier ?study_name ;
+               ro:concretizes ?study_design .
+        ?study_design ro:has_part ?protocol .
+        OPTIONAL {
+            ?protocol ro:has_part ?purposeInst .
+            ?purposeInst a obi:objective_specification ;
+                         cmeo:has_value ?purpose .
+        }
+        OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+        }
+        FILTER(
+            (BOUND(?purpose) &amp;&amp; regex(lcase(str(?purpose)), "diabetes")) ||
+            (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), "diabetes"))
+        )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?description
+WHERE { 
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name;
+            iao:is_about ?descriptor;
+            ro:has_part ?prot .
+        ?descriptor rdfs:label ?description.
+        ?prot a obi:protocol;
+          ro:has_part ?obj_spec.
+        ?obj_spec a obi:objective_specification ;
+            cmeo:has_value ?obj_val.
+        ?prot ro:has_part ?ec.
+        ?ec a obi:eligibility_criterion;
+            ro:has_part ?inc.
+        ?inc a obi:inclusion_criterion;
+            ro:has_part ?spec_inc.
+        ?spec_inc  cmeo:has_value ?inc_value.
+    FILTER(contains(lcase(str(?obj_val)), "diabetes") || contains(lcase(str(?inc_value)), "diabetes"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name;
+                ro:concretizes ?study_design.
+          ?study_design  ro:has_part ?protocol .
+         # Primary purpose specification
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         # Inclusion criteria pattern (optional)
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         # Filter: Only include studies where the primary purpose or inclusion criteria contain "coronary heart disease"
+         FILTER( regex(lcase(str(?purpose)), 'coronary heart disease') ||
+           (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'coronary heart disease'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name ;
+                ro:concretizes ?study_design .
+         ?study_design ro:has_part ?protocol .
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         FILTER( regex(lcase(str(?purpose)), 'coronary heart disease') ||
+                 (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'coronary heart disease'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?description
+WHERE { 
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name;
+            iao:is_about ?descriptor;
+            ro:has_part ?prot .
+        ?descriptor rdfs:label ?description.
+        ?prot a obi:protocol;
+              ro:has_part ?obj_spec.
+        ?obj_spec a obi:objective_specification ;
+                  cmeo:has_value ?obj_val.
+        ?prot ro:has_part ?ec.
+        ?ec a obi:eligibility_criterion;
+            ro:has_part ?inc.
+        ?inc a obi:inclusion_criterion;
+             ro:has_part ?spec_inc.
+        ?spec_inc  cmeo:has_value ?inc_value.
+        FILTER(contains(lcase(str(?obj_val)), "coronary heart disease") || contains(lcase(str(?inc_value)), "coronary heart disease"))
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?description
+WHERE { 
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name;
+            iao:is_about ?descriptor;
+            ro:has_part ?prot .
+        ?descriptor rdfs:label ?description.
+        ?prot a obi:protocol;
+          ro:has_part ?obj_spec.
+        ?obj_spec a obi:objective_specification ;
+            cmeo:has_value ?obj_val.
+        ?prot ro:has_part ?ec.
+        ?ec a obi:eligibility_criterion;
+            ro:has_part ?inc.
+        ?inc a obi:inclusion_criterion;
+            ro:has_part ?spec_inc.
+        ?spec_inc  cmeo:has_value ?inc_value.
+    FILTER(contains(lcase(str(?obj_val)), "coronary heart disease") || contains(lcase(str(?inc_value)), "coronary heart disease"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?variable) AS ?variable_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a obi:study_design_execution ;
+           dc:identifier "time-chf" ;
+           ro:concretizes ?study_design .
+    ?study_design ro:has_part ?protocol .
+    ?protocol ro:has_part ?study_var_design .
+    ?study_var_design a cmeo:study_design_variable_specification ;
+                      ro:has_part ?variable .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?data_element) AS ?variable_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study a obi:study_design_execution ;
+             dc:identifier "time-chf" ;
+             ro:concretizes ?study_design .
+      ?study_design ro:has_part ?protocol .
+      ?protocol ro:has_part ?study_var_design .
+      ?study_var_design a cmeo:study_design_variable_specification ;
+                        ro:has_part ?data_element .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?data_element) AS ?variable_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study a obi:study_design_execution ;
+             dc:identifier "time-chf" ;
+             ro:concretizes ?study_design .
+      ?study_design ro:has_part ?protocol .
+      ?protocol ro:has_part ?study_var_design .
+      ?study_var_design a cmeo:study_design_variable_specification ;
+                        ro:has_part ?data_element .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX cmeo: &lt;https://w3id.org/CMEO/&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt; 
+SELECT (COUNT(?data_element) AS ?var_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study a obi:study_design_execution;
+             dc:identifier "time-chf";
+             ro:concretizes ?study_design.
+      ?study_design ro:has_part ?protocol.
+      ?protocol ro:has_part ?study_var_design.
+      ?study_var_design a cmeo:study_design_variable_specification;
+                        ro:has_part ?data_element.
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?drug_variable) AS ?drug_var_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a obi:study_design_execution ;
+           dc:identifier "time-chf" ;
+           ro:concretizes ?study_design .
+    ?study_design ro:has_part ?protocol .
+    ?protocol ro:has_part ?study_var_design .
+    ?study_var_design a cmeo:study_design_variable_specification ;
+                      ro:has_part ?drug_variable .
+    ?drug_variable cmeo:has_value ?value .
+    FILTER(CONTAINS(LCASE(STR(?value)), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?data_element) AS ?drug_var_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a obi:study_design_execution ;
+           dc:identifier "time-chf" ;
+           ro:concretizes ?study_design .
+    ?study_design ro:has_part ?protocol .
+    ?protocol ro:has_part ?study_var_design .
+    ?study_var_design a cmeo:study_design_variable_specification ;
+                      ro:has_part ?data_element .
+    ?data_element cmeo:has_value ?value .
+    FILTER(regex(lcase(str(?value)), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?data_element) AS ?drug_var_count)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a obi:study_design_execution ;
+           dc:identifier "time-chf" ;
+           ro:concretizes ?study_design .
+    ?study_design ro:has_part ?protocol .
+    ?protocol ro:has_part ?study_var_design .
+    ?study_var_design a cmeo:study_design_variable_specification ;
+                      ro:has_part ?data_element .
+    ?data_element cmeo:has_value ?value .
+    FILTER (regex(lcase(str(?value)), "drug"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT (COUNT(?data_element) AS ?drug_var_count)
+WHERE {
+   GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    	?study a obi:study_design_execution;
+          		dc:identifier "time-chf";
+    			ro:concretizes ?study_design .
+         ?study_design ro:has_part ?protocol .
+         ?protocol ro:has_part ?study_var_design .
+	     ?study_var_design a cmeo:study_design_variable_specification;
+              ro:has_part ?data_element .
+         ?data_element cmeo:has_value ?var_value .
+         FILTER( regex(lcase(str(?var_value)), "drug") )
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?trial_identifier ?protocol ?protocol_part ?protocol_value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?trial a cmeo:randomized_controlled_trial ;
+           dc:identifier ?trial_identifier ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?protocol_part .
+    OPTIONAL { ?protocol_part cmeo:has_value ?protocol_value }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?protocol ?protocol_part ?protocol_value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_name ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?protocol_part .
+    OPTIONAL { ?protocol_part cmeo:has_value ?protocol_value . }
+  }
+}
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?protocol ?protocol_part ?protocol_value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_name ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?protocol_part .
+    OPTIONAL { ?protocol_part cmeo:has_value ?protocol_value . }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?protocol ?protocol_part ?protocol_value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study_design a cmeo:randomized_controlled_trial ;
+                  dc:identifier ?study_name ;
+                  ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?protocol_part .
+    OPTIONAL { ?protocol_part cmeo:has_value ?protocol_value . }
+  }
+}
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name ;
+                      ro:has_part ?protocol .
+        ?protocol a obi:protocol ;
+                  ro:has_part ?eligibility_criterion .
+        ?eligibility_criterion a obi:eligibility_criterion ;
+                               ro:has_part ?inclusion_criterion .
+        ?inclusion_criterion a obi:inclusion_criterion ;
+                             ro:has_part ?health_status_inclusion .
+        ?health_status_inclusion a obi:health_status_inclusion_criterion ;
+                                 cmeo:has_value ?condition_value .
+        FILTER(CONTAINS(LCASE(?condition_value), "heart failure"))
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study_design a cmeo:randomized_controlled_trial ;
+                  dc:identifier ?study_name ;
+                  ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility_criterion .
+    ?eligibility_criterion a obi:eligibility_criterion ;
+                           ro:has_part ?inclusion_criterion .
+    ?inclusion_criterion a obi:inclusion_criterion ;
+                         ro:has_part ?health_status_criterion .
+    ?health_status_criterion a obi:health_status_inclusion_criterion ;
+                             cmeo:has_value ?condition_value .
+    FILTER(CONTAINS(LCASE(STR(?condition_value)), "heart failure"))
+  }
+}
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?condition
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a obi:study_design_execution ;
+           dc:identifier ?study_name ;
+           ro:concretizes ?study_design .
+    ?study_design ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility_criterion .
+    ?eligibility_criterion a obi:eligibility_criterion ;
+                           ro:has_part ?inclusion_criterion .
+    ?inclusion_criterion a obi:inclusion_criterion ;
+                         ro:has_part ?health_status_criterion .
+    ?health_status_criterion a obi:health_status_inclusion_criterion ;
+                             cmeo:has_value ?condition .
+    FILTER (regex(lcase(str(?condition)), "heart failure"))
+  }
+}
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?purpose ?inclusion
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+         ?study a obi:study_design_execution ;
+                dc:identifier ?study_name;
+                ro:concretizes ?study_design.
+          ?study_design  ro:has_part ?protocol .
+         # Primary purpose specification
+         ?protocol ro:has_part ?purposeInst .
+         ?purposeInst a obi:objective_specification ;
+                      cmeo:has_value ?purpose .
+         # Inclusion criteria pattern (optional)
+         OPTIONAL {
+            ?protocol ro:has_part ?inclusionInst .
+            ?inclusionInst a obi:inclusion_criterion ;
+                           cmeo:has_value ?inclusion .
+         }
+         # Filter: Only include studies where the primary purpose or inclusion criteria contain "heart failure"
+         FILTER( regex(lcase(str(?purpose)), 'heart failure') ||
+           (BOUND(?inclusion) &amp;&amp; regex(lcase(str(?inclusion)), 'heart failure'))
+         )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT
+    ?study_name
+    (GROUP_CONCAT(DISTINCT COALESCE(?char_value); separator=";") AS ?population_characteristics)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study dc:identifier ?study_name ;
+             ro:has_part ?eligibility_criterion .
+      ?eligibility_criterion a obi:eligibility_criterion ;
+                             ro:has_part ?inclusion_criterion .
+      ?inclusion_criterion a obi:inclusion_criterion ;
+                           ro:has_part ?char .
+      ?char cmeo:has_value ?char_value .
+  }
+}
+GROUP BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT 
+    ?study_name
+    (GROUP_CONCAT(DISTINCT LCASE(STR(?population_value)); SEPARATOR="; ") AS ?population_characteristics)
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study dc:identifier ?study_name ;
+               ro:has_part ?protocol .
+        ?protocol a obi:protocol ;
+                  ro:has_part ?eligibility_criterion .
+        ?eligibility_criterion a obi:eligibility_criterion ;
+                               ro:has_part ?inclusion_criterion .
+        ?inclusion_criterion a obi:inclusion_criterion ;
+                             ro:has_part ?population_part .
+        ?population_part cmeo:has_value ?population_value .
+    }
+}
+GROUP BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name
+(GROUP_CONCAT(DISTINCT LCASE(STR(?diagnosis_value)); separator="; ") AS ?health_status)
+(GROUP_CONCAT(DISTINCT CONCAT("min_age:", STR(?min_val)); separator="; ") AS ?minimum_age)
+(GROUP_CONCAT(DISTINCT CONCAT("max_age:", STR(?max_val)); separator="; ") AS ?maximum_age)
+(GROUP_CONCAT(DISTINCT LCASE(STR(?sex_value)); separator="; ") AS ?sex)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study a cmeo:randomized_controlled_trial ;
+           dc:identifier ?study_name ;
+           ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?eligibility_criterion .
+    ?eligibility_criterion a obi:eligibility_criterion ;
+                           ro:has_part ?inclusion_criterion .
+    ?inclusion_criterion a obi:inclusion_criterion ;
+                         ro:has_part ?inc_part .
+    OPTIONAL {
+      ?inc_part a obi:health_status_inclusion_criterion ;
+                cmeo:has_value ?diagnosis_value .
+    }
+    OPTIONAL {
+      ?inc_part a obi:age_group_inclusion_criterion ;
+                ro:has_part ?min_age_spec, ?max_age_spec .
+      ?min_age_spec a obi:minimum_age_value_specification ;
+                    cmeo:has_value ?min_val .
+      ?max_age_spec a obi:maximum_age_value_specification ;
+                    cmeo:has_value ?max_val .
+    }
+    OPTIONAL {
+      ?inc_part a obi:sex_inclusion_criterion ;
+                cmeo:has_value ?sex_value .
+    }
+  }
+}
+GROUP BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name
+(GROUP_CONCAT(DISTINCT LCASE(STR(?population_value)); SEPARATOR="; ") AS ?population_characteristics)
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study a obi:study_design_execution ;
+             dc:identifier ?study_name ;
+             ro:concretizes ?study_design .
+      ?study_design ro:has_part ?protocol .
+      ?protocol a obi:protocol ;
+                ro:has_part ?eligibility_criterion .
+      ?eligibility_criterion a obi:eligibility_criterion ;
+                ro:has_part ?inclusion_criterion .
+      ?inclusion_criterion a obi:inclusion_criterion ;
+                ro:has_part ?inc_part .
+      ?inc_part cmeo:has_value ?population_value .
+  }
+}
+GROUP BY ?study_name
+ORDER BY ?study_name</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?population ?intervention ?comparator ?outcome
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name ;
+                      ro:has_part ?protocol .
+        ?protocol a obi:protocol ;
+                  ro:has_part ?pop_spec, ?int_spec, ?comp_spec, ?out_spec .
+        ?pop_spec a obi:eligibility_criterion ;
+                  cmeo:has_value ?population .
+        ?int_spec a cmeo:intervention_specification ;
+                  cmeo:has_value ?intervention .
+        ?comp_spec a cmeo:comparator_specification ;
+                   cmeo:has_value ?comparator .
+        ?out_spec a cmeo:outcome_specification ;
+                  cmeo:has_value ?outcome .
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?population ?intervention ?comparator ?outcome
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study_design dc:identifier ?study_name ;
+                  ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?pop_spec, ?int_spec, ?comp_spec, ?out_spec .
+    ?pop_spec a obi:eligibility_criterion ;
+              cmeo:has_value ?population .
+    ?int_spec a cmeo:intervention_specification ;
+              cmeo:has_value ?intervention .
+    ?comp_spec a cmeo:comparator_specification ;
+               cmeo:has_value ?comparator .
+    ?out_spec a cmeo:outcome_specification ;
+              cmeo:has_value ?outcome .
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?population_value ?intervention_value ?comparator_value ?outcome_value
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study_design dc:identifier ?study_name ;
+                  ro:has_part ?protocol .
+    ?protocol a obi:protocol ;
+              ro:has_part ?pop_spec, ?int_spec, ?comp_spec, ?out_spec .
+    OPTIONAL {
+      ?pop_spec a obi:eligibility_criterion ;
+                cmeo:has_value ?population_value .
+    }
+    OPTIONAL {
+      ?int_spec a cmeo:intervention_specification ;
+                cmeo:has_value ?intervention_value .
+    }
+    OPTIONAL {
+      ?comp_spec a cmeo:comparator_specification ;
+                 cmeo:has_value ?comparator_value .
+    }
+    OPTIONAL {
+      ?out_spec a cmeo:outcome_specification ;
+                cmeo:has_value ?outcome_value .
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?population ?intervention ?comparator ?outcome
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+      ?study_design dc:identifier ?study_name ;
+                    ro:has_part ?protocol .
+      ?protocol a obi:protocol ;
+                ro:has_part ?part .
+      OPTIONAL {
+          ?part a obi:eligibility_criterion ;
+                ro:has_part ?inc .
+          ?inc a obi:inclusion_criterion ;
+                cmeo:has_value ?population .
+      }
+      OPTIONAL {
+          ?part a cmeo:intervention_specification ;
+                cmeo:has_value ?intervention .
+      }
+      OPTIONAL {
+          ?part a cmeo:comparator_specification ;
+                cmeo:has_value ?comparator .
+      }
+      OPTIONAL {
+          ?part a cmeo:outcome_specification ;
+                cmeo:has_value ?outcome .
+      }
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?data_permission ?data_modifier
+WHERE {
+  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+    ?study_design dc:identifier ?study_name ;
+                  iao:is_about ?descriptor ;
+                  ro:has_part ?protocol .
+    ?descriptor rdfs:label ?description .
+    ?protocol a obi:protocol ;
+              ro:has_part ?objective_specification .
+    ?objective_specification a obi:objective_specification ;
+                             cmeo:has_value ?objective_value .
+    ?protocol ro:has_part ?data_policy ;
+              ro:has_part ?data_modifier_node .
+    ?data_policy a duo:data_use_permission ;
+                 rdfs:label ?data_permission .
+    ?data_modifier_node a duo:data_use_modifier ;
+                        rdfs:label ?data_modifier .
+    FILTER (contains(lcase(?objective_value), "congestive heart failure"))
+    FILTER (contains(lcase(?data_permission), "disease specific research"))
+    FILTER (contains(lcase(?data_modifier), "ethics approval required"))
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?permission_label ?modifier_label
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study a obi:study_design_execution ;
+               dc:identifier ?study_name ;
+               ro:concretizes ?study_design .
+        ?study_design ro:has_part ?protocol .
+        ?protocol a obi:protocol ;
+                  ro:has_part ?objective_spec .
+        ?objective_spec a obi:objective_specification ;
+                        cmeo:has_value ?objective_value .
+        ?data_policy a duo:data_use_permission ;
+                     rdfs:label ?permission_label .
+        ?data_modifier a duo:data_use_modifier ;
+                       rdfs:label ?modifier_label .
+        FILTER( regex(lcase(str(?objective_value)), "congestive heart failure") &amp;&amp;
+                regex(lcase(str(?permission_label)), "research") &amp;&amp;
+                regex(lcase(str(?modifier_label)), "ethics approval required") )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?permission_label ?modifier_label
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study_design dc:identifier ?study_name ;
+                      iao:is_about ?descriptor ;
+                      ro:has_part ?protocol .
+        ?descriptor rdfs:label ?descriptor_label .
+        ?protocol a obi:protocol ;
+                  ro:has_part ?data_policy ;
+                  ro:has_part ?data_modifier .
+        ?data_policy a duo:data_use_permission ;
+                     rdfs:label ?permission_label .
+        ?data_modifier a duo:data_use_modifier ;
+                       rdfs:label ?modifier_label .
+        FILTER( regex(lcase(str(?descriptor_label)), "congestive heart failure") &amp;&amp;
+                regex(lcase(str(?permission_label)), "research") &amp;&amp;
+                regex(lcase(str(?modifier_label)), "ethics approval") )
+    }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
+PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
+PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
+PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
+PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
+PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
+PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
+PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
+PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
+PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
+PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
+PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
+PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
+SELECT DISTINCT ?study_name ?permission_label ?modifier_label
+WHERE {
+    GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
+        ?study a obi:study_design_execution ;
+               dc:identifier ?study_name ;
+               ro:concretizes ?study_design .
+        ?study_design ro:has_part ?protocol .
+        ?protocol ro:has_part ?objective_spec .
+        ?objective_spec a obi:objective_specification ;
+                        cmeo:has_value ?objective_value .
+        ?protocol ro:has_part ?data_policy .
+        ?data_policy a duo:data_use_permission ;
+                     rdfs:label ?permission_label .
+        ?protocol ro:has_part ?data_modifier .
+        ?data_modifier a duo:data_use_modifier ;
+                       rdfs:label ?modifier_label .
+        FILTER (regex(lcase(str(?objective_value)), "congestive heart failure"))
+        FILTER (regex(lcase(str(?permission_label)), "research"))
+        FILTER (regex(lcase(str(?modifier_label)), "ethics approval"))
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -724,14 +2226,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.26953125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" customWidth="1"/>
     <col min="7" max="7" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -765,11 +2270,21 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -779,11 +2294,21 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -792,11 +2317,21 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -805,11 +2340,21 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -818,11 +2363,21 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -831,6 +2386,21 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -839,6 +2409,21 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -847,6 +2432,21 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -854,6 +2454,21 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BFS traversal for nhop + 50 percent experiments complete
</commit_message>
<xml_diff>
--- a/experiments/results/fewshot_eval.xlsx
+++ b/experiments/results/fewshot_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32472\Desktop\MaastrichtUni\Year3\ThesisSep\CodeDataFinal\nl2sparql-thesis\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754F42F8-213D-4439-A98B-E95DA3A0C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3883E767-2734-490A-A29B-26556EAFECAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="19200" windowHeight="12630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>query_id</t>
   </si>
@@ -399,257 +399,6 @@
   }
 }
 ORDER BY ?study_name</t>
-  </si>
-  <si>
-    <t>only_schema</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT DISTINCT ?study ?disease
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           iao:is_about ?descriptor .
-    ?descriptor cmeo:has_value ?disease .
-    FILTER(CONTAINS(LCASE(?disease), "diabetes"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT DISTINCT ?study ?disease_label
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           iao:is_about ?descriptor .
-    ?descriptor cmeo:has_value ?disease_label .
-    FILTER(CONTAINS(LCASE(?disease_label), "coronary heart disease"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT (COUNT(?variable) AS ?variable_count)
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:study_design_variable_specification ;
-           dc:identifier ?id ;
-           ro:has_part ?variable .
-    FILTER(CONTAINS(LCASE(STR(?id)), "time-chf"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT (COUNT(?variable) AS ?drugVariableCount)
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:study_design_variable_specification ;
-           dc:identifier "time-chf"^^xsd:string ;
-           ro:has_part ?variable .
-    ?variable cmeo:has_value ?value .
-    FILTER(CONTAINS(LCASE(STR(?value)), "drug"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT ?trial ?protocol
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?trial a cmeo:randomized_controlled_trial ;
-           ro:has_part ?protocol .
-    ?protocol a obi:protocol .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT DISTINCT ?study ?study_label
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           iao:is_about ?descriptor ;
-           rdfs:label ?study_label .
-    ?descriptor cmeo:has_value ?condition_value .
-    FILTER(CONTAINS(LCASE(STR(?condition_value)), "heart failure"))
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT ?study ?populationCharacteristic ?value
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           ro:has_part ?eligibilityCriterion .
-    ?eligibilityCriterion a obi:eligibility_criterion ;
-           ro:has_part ?inclusionCriterion .
-    ?inclusionCriterion a obi:inclusion_criterion ;
-           ro:has_part ?populationCharacteristic .
-    ?populationCharacteristic cmeo:has_value ?value .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT DISTINCT ?study ?study_label
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           rdfs:label ?study_label ;
-           ro:has_part ?protocol .
-    ?protocol a obi:protocol ;
-              ro:has_part ?eligibility_criterion, ?intervention, ?comparator, ?outcome .
-    ?eligibility_criterion a obi:eligibility_criterion .
-    ?intervention a cmeo:intervention_specification .
-    ?comparator a cmeo:comparator_specification .
-    ?outcome a cmeo:outcome_specification .
-  }
-}</t>
-  </si>
-  <si>
-    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt; 
-PREFIX dc: &lt;http://purl.org/dc/elements/1.1/&gt;
-PREFIX bfo: &lt;http://purl.obolibrary.org/obo/bfo.owl/&gt;
-PREFIX obi: &lt;http://purl.obolibrary.org/obo/obi.owl/&gt;
-PREFIX ro: &lt;http://purl.obolibrary.org/obo/ro.owl/&gt;
-PREFIX iao: &lt;http://purl.obolibrary.org/obo/iao.owl/&gt;
-PREFIX sio: &lt;http://semanticscience.org/ontology/sio.owl/&gt; 
-PREFIX duo: &lt;http://purl.obolibrary.org/obo/duo/&gt;
-PREFIX obcs: &lt;http://purl.obolibrary.org/obo/obcs.owl/&gt; 
-PREFIX stato: &lt;http://purl.obolibrary.org/obo/stato.owl/&gt;
-PREFIX cdi: &lt;http://ddialliance.org/Specification/DDI-CDI/1.0/RDF/&gt;
-PREFIX cd: &lt;http://citydata.wu.ac.at/ns#&gt;
-PREFIX cmeo: &lt;https://w3id.org/cmeo/&gt;
-SELECT DISTINCT ?study
-WHERE {
-  GRAPH &lt;https://w3id.org/CMEO/graph/studies_metadata&gt; {
-    ?study a cmeo:randomized_controlled_trial ;
-           iao:is_about ?descriptor ;
-           ro:has_part ?data_policy , ?data_modifier .
-    ?data_policy a duo:data_use_permission ;
-                 rdfs:label "disease specific research"^^xsd:string .
-    ?data_modifier a duo:data_use_modifier ;
-                   rdfs:label "ethics approval required"^^xsd:string .
-    ?descriptor cmeo:has_value ?disease .
-    FILTER(CONTAINS(LCASE(?disease), "congestive heart failure"))
-  }
-}</t>
   </si>
   <si>
     <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
@@ -2224,23 +1973,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="39.453125" customWidth="1"/>
-    <col min="7" max="7" width="25.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="5" max="5" width="39.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2248,22 +1996,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2271,23 +2016,20 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2295,22 +2037,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2318,22 +2057,19 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2341,22 +2077,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2364,22 +2097,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2387,22 +2117,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2410,22 +2137,19 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2433,22 +2157,19 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2456,19 +2177,16 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>